<commit_message>
clean project table for dashboard 2
</commit_message>
<xml_diff>
--- a/reference_data/list_implementors_categories.xlsx
+++ b/reference_data/list_implementors_categories.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nruddle\Dropbox (OPML)\A2241 MAINTAINS\TA - Finance tracking\Analysis\analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repositaries\1.work\ERP\reference_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{915F4555-DBAE-49B9-9AA8-85F695031AD6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A91C5DE1-E351-4C1D-B433-57728E1ACB4E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="178">
   <si>
     <t>Implementor</t>
   </si>
@@ -548,6 +548,12 @@
   </si>
   <si>
     <t>Oxford Policy Management</t>
+  </si>
+  <si>
+    <t>Oxfam Novip (Netherlands)</t>
+  </si>
+  <si>
+    <t>Oxfam Uganda</t>
   </si>
 </sst>
 </file>
@@ -899,18 +905,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C85"/>
+  <dimension ref="A1:C87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
-      <selection activeCell="B86" sqref="B86"/>
+    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
+      <selection activeCell="B90" sqref="B90"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="74.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="74.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -918,7 +924,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -929,7 +935,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -940,7 +946,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -951,7 +957,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -962,7 +968,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -973,7 +979,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -984,7 +990,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -995,7 +1001,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -1006,7 +1012,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -1017,7 +1023,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -1028,7 +1034,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1039,7 +1045,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -1050,7 +1056,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -1061,7 +1067,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -1072,7 +1078,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -1083,7 +1089,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -1094,7 +1100,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -1105,7 +1111,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -1116,7 +1122,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -1127,7 +1133,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -1138,7 +1144,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -1149,7 +1155,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -1160,7 +1166,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -1171,7 +1177,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -1182,7 +1188,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -1193,7 +1199,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -1204,7 +1210,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -1215,7 +1221,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -1226,7 +1232,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -1237,7 +1243,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -1248,7 +1254,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>31</v>
       </c>
@@ -1259,7 +1265,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>32</v>
       </c>
@@ -1270,7 +1276,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>33</v>
       </c>
@@ -1281,7 +1287,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>34</v>
       </c>
@@ -1292,7 +1298,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>35</v>
       </c>
@@ -1303,7 +1309,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>36</v>
       </c>
@@ -1314,7 +1320,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>37</v>
       </c>
@@ -1325,7 +1331,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>38</v>
       </c>
@@ -1336,7 +1342,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>39</v>
       </c>
@@ -1347,7 +1353,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>40</v>
       </c>
@@ -1358,7 +1364,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>41</v>
       </c>
@@ -1369,7 +1375,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>42</v>
       </c>
@@ -1380,7 +1386,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>43</v>
       </c>
@@ -1391,7 +1397,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>44</v>
       </c>
@@ -1402,7 +1408,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>45</v>
       </c>
@@ -1413,7 +1419,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>46</v>
       </c>
@@ -1424,7 +1430,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>47</v>
       </c>
@@ -1435,7 +1441,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>48</v>
       </c>
@@ -1446,7 +1452,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>49</v>
       </c>
@@ -1457,7 +1463,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>50</v>
       </c>
@@ -1468,7 +1474,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>51</v>
       </c>
@@ -1479,7 +1485,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>52</v>
       </c>
@@ -1490,7 +1496,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>53</v>
       </c>
@@ -1501,7 +1507,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>54</v>
       </c>
@@ -1512,7 +1518,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>55</v>
       </c>
@@ -1523,7 +1529,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>56</v>
       </c>
@@ -1534,7 +1540,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>57</v>
       </c>
@@ -1545,7 +1551,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>58</v>
       </c>
@@ -1556,7 +1562,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>59</v>
       </c>
@@ -1567,7 +1573,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>60</v>
       </c>
@@ -1578,7 +1584,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>61</v>
       </c>
@@ -1589,7 +1595,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>62</v>
       </c>
@@ -1600,7 +1606,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>63</v>
       </c>
@@ -1611,7 +1617,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>64</v>
       </c>
@@ -1622,7 +1628,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>65</v>
       </c>
@@ -1633,7 +1639,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>66</v>
       </c>
@@ -1644,7 +1650,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>67</v>
       </c>
@@ -1655,7 +1661,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>68</v>
       </c>
@@ -1666,7 +1672,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>69</v>
       </c>
@@ -1677,7 +1683,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>70</v>
       </c>
@@ -1688,7 +1694,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>71</v>
       </c>
@@ -1699,7 +1705,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>72</v>
       </c>
@@ -1710,7 +1716,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>73</v>
       </c>
@@ -1721,7 +1727,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>74</v>
       </c>
@@ -1732,7 +1738,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>75</v>
       </c>
@@ -1743,7 +1749,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>76</v>
       </c>
@@ -1754,7 +1760,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>77</v>
       </c>
@@ -1765,7 +1771,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>78</v>
       </c>
@@ -1776,7 +1782,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>79</v>
       </c>
@@ -1787,7 +1793,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>80</v>
       </c>
@@ -1798,7 +1804,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>81</v>
       </c>
@@ -1809,7 +1815,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>82</v>
       </c>
@@ -1820,7 +1826,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>83</v>
       </c>
@@ -1831,7 +1837,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>84</v>
       </c>
@@ -1840,6 +1846,28 @@
       </c>
       <c r="C85" t="s">
         <v>174</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A86">
+        <v>85</v>
+      </c>
+      <c r="B86" t="s">
+        <v>176</v>
+      </c>
+      <c r="C86" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A87">
+        <v>86</v>
+      </c>
+      <c r="B87" t="s">
+        <v>177</v>
+      </c>
+      <c r="C87" t="s">
+        <v>170</v>
       </c>
     </row>
   </sheetData>

</xml_diff>